<commit_message>
Add texture names and adjust scale for fall tree textures
</commit_message>
<xml_diff>
--- a/resource/textures/texture-index.xlsx
+++ b/resource/textures/texture-index.xlsx
@@ -4274,9 +4274,6 @@
     <t>fall leaves 9 replaces #8865</t>
   </si>
   <si>
-    <t>fall leaves 10 replaces #9766 and #10000</t>
-  </si>
-  <si>
     <t>fall leaves 11 replaces #8861</t>
   </si>
   <si>
@@ -4287,6 +4284,9 @@
   </si>
   <si>
     <t>fall leaves 14 replaces #8864</t>
+  </si>
+  <si>
+    <t>fall leaves 10 replaces #9776 and #10000</t>
   </si>
 </sst>
 </file>
@@ -4664,8 +4664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1435"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1403" workbookViewId="0">
-      <selection activeCell="B1436" sqref="B1436"/>
+    <sheetView tabSelected="1" topLeftCell="A1400" workbookViewId="0">
+      <selection activeCell="B1421" sqref="B1421"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16119,7 +16119,7 @@
         <v>61027</v>
       </c>
       <c r="B1431" s="1" t="s">
-        <v>1413</v>
+        <v>1417</v>
       </c>
     </row>
     <row r="1432" spans="1:2" x14ac:dyDescent="0.25">
@@ -16127,7 +16127,7 @@
         <v>61028</v>
       </c>
       <c r="B1432" s="1" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
     </row>
     <row r="1433" spans="1:2" x14ac:dyDescent="0.25">
@@ -16135,7 +16135,7 @@
         <v>61029</v>
       </c>
       <c r="B1433" s="1" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
     </row>
     <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
@@ -16143,7 +16143,7 @@
         <v>61030</v>
       </c>
       <c r="B1434" s="1" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
     </row>
     <row r="1435" spans="1:2" x14ac:dyDescent="0.25">
@@ -16151,7 +16151,7 @@
         <v>61031</v>
       </c>
       <c r="B1435" s="1" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
     </row>
   </sheetData>

</xml_diff>